<commit_message>
fixed error files - removed padding
</commit_message>
<xml_diff>
--- a/predicted.xlsx
+++ b/predicted.xlsx
@@ -479,7 +479,7 @@
         <v>0.0106693292036652</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01028368794326241</v>
+        <v>0.01065292096219931</v>
       </c>
     </row>
     <row r="3">
@@ -501,7 +501,7 @@
         <v>0.008626070804893899</v>
       </c>
       <c r="F3" t="n">
-        <v>0.009278350515463918</v>
+        <v>0.008591065292096219</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +545,7 @@
         <v>0.008052365854382499</v>
       </c>
       <c r="F5" t="n">
-        <v>0.007317073170731708</v>
+        <v>0.008013937282229966</v>
       </c>
     </row>
     <row r="6">
@@ -567,7 +567,7 @@
         <v>0.0106693292036652</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01029159519725557</v>
+        <v>0.01132075471698113</v>
       </c>
     </row>
     <row r="7">
@@ -589,7 +589,7 @@
         <v>0.0105183003470301</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01047120418848168</v>
+        <v>0.01047297297297297</v>
       </c>
     </row>
     <row r="8">
@@ -611,7 +611,7 @@
         <v>0.0090076420456171</v>
       </c>
       <c r="F8" t="n">
-        <v>0.008273381294964029</v>
+        <v>0.009326424870466322</v>
       </c>
     </row>
     <row r="9">
@@ -633,7 +633,7 @@
         <v>0.009631616994738501</v>
       </c>
       <c r="F9" t="n">
-        <v>0.009252669039145907</v>
+        <v>0.009605488850771868</v>
       </c>
     </row>
     <row r="10">
@@ -655,7 +655,7 @@
         <v>0.008052365854382499</v>
       </c>
       <c r="F10" t="n">
-        <v>0.007317073170731708</v>
+        <v>0.008362369337979094</v>
       </c>
     </row>
     <row r="11">
@@ -699,7 +699,7 @@
         <v>0.0091118793934583</v>
       </c>
       <c r="F12" t="n">
-        <v>0.007238095238095238</v>
+        <v>0.009411764705882352</v>
       </c>
     </row>
     <row r="13">
@@ -743,7 +743,7 @@
         <v>0.0080036586150527</v>
       </c>
       <c r="F14" t="n">
-        <v>0.007636363636363636</v>
+        <v>0.00798611111111111</v>
       </c>
     </row>
     <row r="15">
@@ -765,7 +765,7 @@
         <v>0.0110701210796833</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01070811744386874</v>
+        <v>0.01105354058721934</v>
       </c>
     </row>
     <row r="16">
@@ -787,7 +787,7 @@
         <v>0.0103474156931042</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0103202846975089</v>
+        <v>0.01030927835051546</v>
       </c>
     </row>
     <row r="17">
@@ -809,7 +809,7 @@
         <v>0.0106693292036652</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01028368794326241</v>
+        <v>0.01063464837049743</v>
       </c>
     </row>
     <row r="18">
@@ -830,7 +830,9 @@
       <c r="E18" t="n">
         <v>0.0073726726695895</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>0.01006944444444445</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -851,7 +853,7 @@
         <v>0.008052365854382499</v>
       </c>
       <c r="F19" t="n">
-        <v>0.007665505226480837</v>
+        <v>0.008013937282229966</v>
       </c>
     </row>
     <row r="20">
@@ -873,7 +875,7 @@
         <v>0.0073580937460064</v>
       </c>
       <c r="F20" t="n">
-        <v>0.006030150753768845</v>
+        <v>0.007342657342657343</v>
       </c>
     </row>
     <row r="21">
@@ -917,7 +919,7 @@
         <v>0.0073726726695895</v>
       </c>
       <c r="F22" t="n">
-        <v>0.007005253940455342</v>
+        <v>0.007355516637478108</v>
       </c>
     </row>
     <row r="23">
@@ -939,7 +941,7 @@
         <v>0.0066928141750395</v>
       </c>
       <c r="F23" t="n">
-        <v>0.001689189189189189</v>
+        <v>0.01045296167247387</v>
       </c>
     </row>
     <row r="24">
@@ -961,7 +963,7 @@
         <v>0.0081770177930593</v>
       </c>
       <c r="F24" t="n">
-        <v>0.009557522123893806</v>
+        <v>0.008141592920353982</v>
       </c>
     </row>
     <row r="25">
@@ -1005,7 +1007,7 @@
         <v>0.0082667367532849</v>
       </c>
       <c r="F26" t="n">
-        <v>0.008823529411764706</v>
+        <v>0.01090289608177172</v>
       </c>
     </row>
     <row r="27">
@@ -1027,7 +1029,7 @@
         <v>0.009348879568278699</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00933572710951526</v>
+        <v>0.009326424870466322</v>
       </c>
     </row>
     <row r="28">
@@ -1049,7 +1051,7 @@
         <v>0.0071303099393844</v>
       </c>
       <c r="F28" t="n">
-        <v>0.004262877442273535</v>
+        <v>0.007815275310834813</v>
       </c>
     </row>
     <row r="29">
@@ -1071,7 +1073,7 @@
         <v>0.0091118793934583</v>
       </c>
       <c r="F29" t="n">
-        <v>0.009563409563409562</v>
+        <v>0.00909090909090909</v>
       </c>
     </row>
     <row r="30">
@@ -1093,7 +1095,7 @@
         <v>0.0073726726695895</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001663893510815308</v>
+        <v>0.01035058430717863</v>
       </c>
     </row>
     <row r="31">
@@ -1158,7 +1160,9 @@
       <c r="E33" t="n">
         <v>0.0033885452430695</v>
       </c>
-      <c r="F33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>0.006137184115523466</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1179,7 +1183,7 @@
         <v>0.0036973746027797</v>
       </c>
       <c r="F34" t="n">
-        <v>0.002735042735042735</v>
+        <v>0.004128440366972477</v>
       </c>
     </row>
     <row r="35">
@@ -1201,7 +1205,7 @@
         <v>0.0061830580234527</v>
       </c>
       <c r="F35" t="n">
-        <v>0.005851979345955249</v>
+        <v>0.006206896551724138</v>
       </c>
     </row>
     <row r="36">
@@ -1223,7 +1227,7 @@
         <v>0.0069400747306644</v>
       </c>
       <c r="F36" t="n">
-        <v>0.006951871657754011</v>
+        <v>0.006930693069306931</v>
       </c>
     </row>
     <row r="37">
@@ -1245,7 +1249,7 @@
         <v>0.0068595996126532</v>
       </c>
       <c r="F37" t="n">
-        <v>0.006859205776173286</v>
+        <v>0.00684931506849315</v>
       </c>
     </row>
     <row r="38">
@@ -1267,7 +1271,7 @@
         <v>0.0047356453724205</v>
       </c>
       <c r="F38" t="n">
-        <v>0.004735883424408015</v>
+        <v>0.00472972972972973</v>
       </c>
     </row>
     <row r="39">
@@ -1289,7 +1293,7 @@
         <v>0.004652583040297</v>
       </c>
       <c r="F39" t="n">
-        <v>0.004659498207885305</v>
+        <v>0.00466786355475763</v>
       </c>
     </row>
     <row r="40">
@@ -1355,7 +1359,7 @@
         <v>0.0094863306730985</v>
       </c>
       <c r="F42" t="n">
-        <v>0.009480812641083521</v>
+        <v>0.009482758620689655</v>
       </c>
     </row>
     <row r="43">
@@ -1399,7 +1403,7 @@
         <v>0.0110701210796833</v>
       </c>
       <c r="F44" t="n">
-        <v>0.01104761904761905</v>
+        <v>0.01104972375690608</v>
       </c>
     </row>
     <row r="45">
@@ -1465,7 +1469,7 @@
         <v>0.0096008023247122</v>
       </c>
       <c r="F47" t="n">
-        <v>0.00920353982300885</v>
+        <v>0.009557522123893806</v>
       </c>
     </row>
     <row r="48">
@@ -1487,7 +1491,7 @@
         <v>0.0073800808750092</v>
       </c>
       <c r="F48" t="n">
-        <v>0.007005253940455342</v>
+        <v>0.007355516637478108</v>
       </c>
     </row>
     <row r="49">
@@ -1508,7 +1512,9 @@
       <c r="E49" t="n">
         <v>0.0073726726695895</v>
       </c>
-      <c r="F49" t="inlineStr"/>
+      <c r="F49" t="n">
+        <v>0.01217391304347826</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1551,7 +1557,7 @@
         <v>0.0105183003470301</v>
       </c>
       <c r="F51" t="n">
-        <v>0.009773123909249563</v>
+        <v>0.01039861351819757</v>
       </c>
     </row>
     <row r="52">
@@ -1573,7 +1579,7 @@
         <v>0.0082667367532849</v>
       </c>
       <c r="F52" t="n">
-        <v>0.008380952380952381</v>
+        <v>0.008235294117647059</v>
       </c>
     </row>
     <row r="53">
@@ -1595,7 +1601,7 @@
         <v>0.0073466841131448</v>
       </c>
       <c r="F53" t="n">
-        <v>0.004333333333333333</v>
+        <v>0.007381370826010545</v>
       </c>
     </row>
     <row r="54">
@@ -1617,7 +1623,7 @@
         <v>0.0122604351490736</v>
       </c>
       <c r="F54" t="n">
-        <v>0.01219512195121951</v>
+        <v>0.01218274111675127</v>
       </c>
     </row>
     <row r="55">
@@ -1639,7 +1645,7 @@
         <v>0.0090076420456171</v>
       </c>
       <c r="F55" t="n">
-        <v>0.008633093525179856</v>
+        <v>0.008981001727115715</v>
       </c>
     </row>
     <row r="56">
@@ -1661,7 +1667,7 @@
         <v>0.0063971159979701</v>
       </c>
       <c r="F56" t="n">
-        <v>0.003202846975088968</v>
+        <v>0.008445945945945945</v>
       </c>
     </row>
     <row r="57">
@@ -1705,7 +1711,7 @@
         <v>0.0081770177930593</v>
       </c>
       <c r="F58" t="n">
-        <v>0.006737588652482269</v>
+        <v>0.008156028368794326</v>
       </c>
     </row>
     <row r="59">
@@ -1727,7 +1733,7 @@
         <v>0.0068595996126532</v>
       </c>
       <c r="F59" t="n">
-        <v>0.006859205776173286</v>
+        <v>0.00684931506849315</v>
       </c>
     </row>
     <row r="60">
@@ -1771,7 +1777,7 @@
         <v>0.01020460110157728</v>
       </c>
       <c r="F61" t="n">
-        <v>0.01029411764705882</v>
+        <v>0.01030195381882771</v>
       </c>
     </row>
     <row r="62">
@@ -1793,7 +1799,7 @@
         <v>0.007358093746006489</v>
       </c>
       <c r="F62" t="n">
-        <v>0.005871559633027523</v>
+        <v>0.008726003490401396</v>
       </c>
     </row>
     <row r="63">
@@ -1815,7 +1821,7 @@
         <v>0.00540638156235218</v>
       </c>
       <c r="F63" t="n">
-        <v>0.005620608899297423</v>
+        <v>0.005385996409335727</v>
       </c>
     </row>
     <row r="64">
@@ -1837,7 +1843,7 @@
         <v>0.009007642045617104</v>
       </c>
       <c r="F64" t="n">
-        <v>0.006837606837606838</v>
+        <v>0.009605488850771868</v>
       </c>
     </row>
     <row r="65">
@@ -1859,7 +1865,7 @@
         <v>0.009450222365558147</v>
       </c>
       <c r="F65" t="n">
-        <v>0.00945709281961471</v>
+        <v>0.009491525423728813</v>
       </c>
     </row>
     <row r="66">
@@ -1881,7 +1887,7 @@
         <v>0.006517439149320126</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0054249547920434</v>
+        <v>0.007521367521367522</v>
       </c>
     </row>
     <row r="67">
@@ -1903,7 +1909,7 @@
         <v>0.01140841282904148</v>
       </c>
       <c r="F67" t="n">
-        <v>0.01261682242990654</v>
+        <v>0.01172413793103448</v>
       </c>
     </row>
     <row r="68">
@@ -1947,7 +1953,7 @@
         <v>0.008177017793059349</v>
       </c>
       <c r="F69" t="n">
-        <v>0.008659793814432989</v>
+        <v>0.008510638297872341</v>
       </c>
     </row>
     <row r="70">
@@ -1969,7 +1975,7 @@
         <v>0.009007642045617104</v>
       </c>
       <c r="F70" t="n">
-        <v>0.009471766848816029</v>
+        <v>0.008981001727115715</v>
       </c>
     </row>
     <row r="71">
@@ -1991,7 +1997,7 @@
         <v>0.009201055392622948</v>
       </c>
       <c r="F71" t="n">
-        <v>0.009152542372881357</v>
+        <v>0.009863945578231292</v>
       </c>
     </row>
     <row r="72">
@@ -2013,7 +2019,7 @@
         <v>0.008177017793059349</v>
       </c>
       <c r="F72" t="n">
-        <v>0.008214285714285714</v>
+        <v>0.008156028368794326</v>
       </c>
     </row>
     <row r="73">
@@ -2035,7 +2041,7 @@
         <v>0.0101357027888298</v>
       </c>
       <c r="F73" t="n">
-        <v>0.01010452961672474</v>
+        <v>0.0101010101010101</v>
       </c>
     </row>
     <row r="74">
@@ -2057,7 +2063,7 @@
         <v>0.00669281417503953</v>
       </c>
       <c r="F74" t="n">
-        <v>0.004511278195488721</v>
+        <v>0.007719298245614034</v>
       </c>
     </row>
     <row r="75">
@@ -2101,7 +2107,7 @@
         <v>0.0101388106122613</v>
       </c>
       <c r="F76" t="n">
-        <v>0.01010452961672474</v>
+        <v>0.0101010101010101</v>
       </c>
     </row>
     <row r="77">
@@ -2123,7 +2129,7 @@
         <v>0.008293010294437408</v>
       </c>
       <c r="F77" t="n">
-        <v>0.005851979345955249</v>
+        <v>0.009294320137693631</v>
       </c>
     </row>
     <row r="78">
@@ -2145,7 +2151,7 @@
         <v>0.01200548838824034</v>
       </c>
       <c r="F78" t="n">
-        <v>0.01202749140893471</v>
+        <v>0.01206030150753769</v>
       </c>
     </row>
     <row r="79">
@@ -2167,7 +2173,7 @@
         <v>0.007380080875009298</v>
       </c>
       <c r="F79" t="n">
-        <v>0.007106598984771573</v>
+        <v>0.007725321888412016</v>
       </c>
     </row>
     <row r="80">
@@ -2189,7 +2195,7 @@
         <v>0.01158675365149975</v>
       </c>
       <c r="F80" t="n">
-        <v>0.01118881118881119</v>
+        <v>0.01154499151103565</v>
       </c>
     </row>
     <row r="81">
@@ -2211,7 +2217,7 @@
         <v>0.0110701210796833</v>
       </c>
       <c r="F81" t="n">
-        <v>0.0106951871657754</v>
+        <v>0.01105354058721934</v>
       </c>
     </row>
     <row r="82">
@@ -2233,7 +2239,7 @@
         <v>0.009201055392622948</v>
       </c>
       <c r="F82" t="n">
-        <v>0.009628008752735229</v>
+        <v>0.01120840630472855</v>
       </c>
     </row>
     <row r="83">
@@ -2277,7 +2283,7 @@
         <v>0.009984917938709259</v>
       </c>
       <c r="F84" t="n">
-        <v>0.00994671403197158</v>
+        <v>0.009948542024013723</v>
       </c>
     </row>
     <row r="85">
@@ -2299,7 +2305,7 @@
         <v>0.009201055392622948</v>
       </c>
       <c r="F85" t="n">
-        <v>0.009168081494057727</v>
+        <v>0.009215017064846417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>